<commit_message>
Refactored some stuff, about to add ID3 tag to MP3 decoder
</commit_message>
<xml_diff>
--- a/docs/LCD/customChars.xlsx
+++ b/docs/LCD/customChars.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicot\OneDrive\Documents\MCUXpressoIDE_10.2.0_759\Micros\TPs\tpf-mp3-player\docs\LCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96810A42-4549-421D-AD3E-F5B34196D433}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8CC124-7F3E-48DD-852F-A6973492124B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2604" yWindow="612" windowWidth="6276" windowHeight="4140" xr2:uid="{2621102A-7D8C-481F-A64A-169C19D7CE1B}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{2621102A-7D8C-481F-A64A-169C19D7CE1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -54,6 +54,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -150,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -167,6 +173,16 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -481,15 +497,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43AA64A4-D781-47F1-9DC0-07FD65ECE894}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:AK12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T7" sqref="T7"/>
+      <selection activeCell="AJ11" sqref="AJ11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData>
-    <row r="1" spans="1:13" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:37" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -500,8 +516,29 @@
       <c r="K1" s="15"/>
       <c r="L1" s="15"/>
       <c r="M1" s="4"/>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="P1" s="17"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="3"/>
+      <c r="T1" s="4"/>
+      <c r="U1" s="25"/>
+      <c r="V1" s="24"/>
+      <c r="W1" s="24"/>
+      <c r="X1" s="24"/>
+      <c r="Y1" s="24"/>
+      <c r="Z1" s="24"/>
+      <c r="AA1" s="25"/>
+      <c r="AC1" s="24"/>
+      <c r="AD1" s="24"/>
+      <c r="AE1" s="24"/>
+      <c r="AF1" s="24"/>
+      <c r="AG1" s="24"/>
+      <c r="AH1" s="24"/>
+      <c r="AI1" s="24"/>
+      <c r="AJ1" s="24"/>
+      <c r="AK1" s="24"/>
+    </row>
+    <row r="2" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="5"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -512,8 +549,29 @@
       <c r="K2" s="10"/>
       <c r="L2" s="1"/>
       <c r="M2" s="13"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="P2" s="18"/>
+      <c r="Q2" s="24"/>
+      <c r="R2" s="16"/>
+      <c r="S2" s="16"/>
+      <c r="T2" s="19"/>
+      <c r="U2" s="25"/>
+      <c r="V2" s="24"/>
+      <c r="W2" s="24"/>
+      <c r="X2" s="24"/>
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="24"/>
+      <c r="AA2" s="25"/>
+      <c r="AC2" s="24"/>
+      <c r="AD2" s="24"/>
+      <c r="AE2" s="24"/>
+      <c r="AF2" s="24"/>
+      <c r="AG2" s="24"/>
+      <c r="AH2" s="24"/>
+      <c r="AI2" s="24"/>
+      <c r="AJ2" s="24"/>
+      <c r="AK2" s="24"/>
+    </row>
+    <row r="3" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="5"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10"/>
@@ -524,8 +582,29 @@
       <c r="K3" s="10"/>
       <c r="L3" s="10"/>
       <c r="M3" s="13"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="P3" s="18"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="24"/>
+      <c r="S3" s="24"/>
+      <c r="T3" s="19"/>
+      <c r="U3" s="25"/>
+      <c r="V3" s="24"/>
+      <c r="W3" s="24"/>
+      <c r="X3" s="24"/>
+      <c r="Y3" s="24"/>
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="25"/>
+      <c r="AC3" s="24"/>
+      <c r="AD3" s="24"/>
+      <c r="AE3" s="24"/>
+      <c r="AF3" s="24"/>
+      <c r="AG3" s="24"/>
+      <c r="AH3" s="24"/>
+      <c r="AI3" s="24"/>
+      <c r="AJ3" s="24"/>
+      <c r="AK3" s="24"/>
+    </row>
+    <row r="4" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="5"/>
       <c r="B4" s="1"/>
       <c r="C4" s="10"/>
@@ -536,8 +615,29 @@
       <c r="K4" s="10"/>
       <c r="L4" s="1"/>
       <c r="M4" s="13"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="P4" s="18"/>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="25"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="24"/>
+      <c r="X4" s="24"/>
+      <c r="Y4" s="24"/>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="25"/>
+      <c r="AC4" s="24"/>
+      <c r="AD4" s="24"/>
+      <c r="AE4" s="24"/>
+      <c r="AF4" s="24"/>
+      <c r="AG4" s="24"/>
+      <c r="AH4" s="24"/>
+      <c r="AI4" s="24"/>
+      <c r="AJ4" s="24"/>
+      <c r="AK4" s="24"/>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="8"/>
       <c r="B5" s="1"/>
       <c r="C5" s="10"/>
@@ -548,8 +648,29 @@
       <c r="K5" s="10"/>
       <c r="L5" s="1"/>
       <c r="M5" s="13"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="P5" s="18"/>
+      <c r="Q5" s="24"/>
+      <c r="R5" s="24"/>
+      <c r="S5" s="24"/>
+      <c r="T5" s="19"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24"/>
+      <c r="X5" s="24"/>
+      <c r="Y5" s="24"/>
+      <c r="Z5" s="24"/>
+      <c r="AA5" s="25"/>
+      <c r="AC5" s="24"/>
+      <c r="AD5" s="24"/>
+      <c r="AE5" s="24"/>
+      <c r="AF5" s="24"/>
+      <c r="AG5" s="24"/>
+      <c r="AH5" s="24"/>
+      <c r="AI5" s="24"/>
+      <c r="AJ5" s="24"/>
+      <c r="AK5" s="24"/>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="8"/>
       <c r="B6" s="1"/>
       <c r="C6" s="10"/>
@@ -560,8 +681,29 @@
       <c r="K6" s="10"/>
       <c r="L6" s="1"/>
       <c r="M6" s="13"/>
-    </row>
-    <row r="7" spans="1:13" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="P6" s="18"/>
+      <c r="Q6" s="24"/>
+      <c r="R6" s="24"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="19"/>
+      <c r="U6" s="25"/>
+      <c r="V6" s="24"/>
+      <c r="W6" s="24"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="24"/>
+      <c r="Z6" s="24"/>
+      <c r="AA6" s="25"/>
+      <c r="AC6" s="24"/>
+      <c r="AD6" s="24"/>
+      <c r="AE6" s="24"/>
+      <c r="AF6" s="24"/>
+      <c r="AG6" s="24"/>
+      <c r="AH6" s="24"/>
+      <c r="AI6" s="24"/>
+      <c r="AJ6" s="24"/>
+      <c r="AK6" s="24"/>
+    </row>
+    <row r="7" spans="1:37" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
       <c r="A7" s="9"/>
       <c r="B7" s="7"/>
       <c r="C7" s="11"/>
@@ -572,15 +714,114 @@
       <c r="K7" s="1"/>
       <c r="L7" s="10"/>
       <c r="M7" s="13"/>
-    </row>
-    <row r="8" spans="1:13" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="P7" s="18"/>
+      <c r="Q7" s="24"/>
+      <c r="R7" s="24"/>
+      <c r="S7" s="24"/>
+      <c r="T7" s="19"/>
+      <c r="U7" s="25"/>
+      <c r="V7" s="24"/>
+      <c r="W7" s="24"/>
+      <c r="X7" s="24"/>
+      <c r="Y7" s="24"/>
+      <c r="Z7" s="24"/>
+      <c r="AA7" s="25"/>
+      <c r="AC7" s="24"/>
+      <c r="AD7" s="24"/>
+      <c r="AE7" s="24"/>
+      <c r="AF7" s="24"/>
+      <c r="AG7" s="24"/>
+      <c r="AH7" s="24"/>
+      <c r="AI7" s="24"/>
+      <c r="AJ7" s="24"/>
+      <c r="AK7" s="24"/>
+    </row>
+    <row r="8" spans="1:37" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
       <c r="L8" s="11"/>
       <c r="M8" s="14"/>
-    </row>
-    <row r="9" spans="1:13" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004"/>
+      <c r="P8" s="20"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="25"/>
+      <c r="V8" s="24"/>
+      <c r="W8" s="24"/>
+      <c r="X8" s="24"/>
+      <c r="Y8" s="24"/>
+      <c r="Z8" s="24"/>
+      <c r="AA8" s="25"/>
+      <c r="AC8" s="24"/>
+      <c r="AD8" s="24"/>
+      <c r="AE8" s="24"/>
+      <c r="AF8" s="24"/>
+      <c r="AG8" s="24"/>
+      <c r="AH8" s="24"/>
+      <c r="AI8" s="24"/>
+      <c r="AJ8" s="24"/>
+      <c r="AK8" s="24"/>
+    </row>
+    <row r="9" spans="1:37" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="U9" s="25"/>
+      <c r="V9" s="24"/>
+      <c r="W9" s="24"/>
+      <c r="X9" s="24"/>
+      <c r="Y9" s="24"/>
+      <c r="Z9" s="24"/>
+      <c r="AA9" s="25"/>
+      <c r="AC9" s="24"/>
+      <c r="AD9" s="24"/>
+      <c r="AE9" s="24"/>
+      <c r="AF9" s="24"/>
+      <c r="AG9" s="24"/>
+      <c r="AH9" s="24"/>
+      <c r="AI9" s="24"/>
+      <c r="AJ9" s="24"/>
+      <c r="AK9" s="24"/>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="U10" s="25"/>
+      <c r="V10" s="24"/>
+      <c r="W10" s="24"/>
+      <c r="X10" s="24"/>
+      <c r="Y10" s="24"/>
+      <c r="Z10" s="24"/>
+      <c r="AA10" s="25"/>
+      <c r="AC10" s="24"/>
+      <c r="AD10" s="24"/>
+      <c r="AE10" s="24"/>
+      <c r="AF10" s="24"/>
+      <c r="AG10" s="24"/>
+      <c r="AH10" s="24"/>
+      <c r="AI10" s="24"/>
+      <c r="AJ10" s="24"/>
+      <c r="AK10" s="24"/>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC11" s="24"/>
+      <c r="AD11" s="24"/>
+      <c r="AE11" s="24"/>
+      <c r="AF11" s="24"/>
+      <c r="AG11" s="24"/>
+      <c r="AH11" s="24"/>
+      <c r="AI11" s="24"/>
+      <c r="AJ11" s="24"/>
+      <c r="AK11" s="24"/>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+      <c r="AC12" s="24"/>
+      <c r="AD12" s="24"/>
+      <c r="AE12" s="24"/>
+      <c r="AF12" s="24"/>
+      <c r="AG12" s="24"/>
+      <c r="AH12" s="24"/>
+      <c r="AI12" s="24"/>
+      <c r="AJ12" s="24"/>
+      <c r="AK12" s="24"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
logos de play y pause
</commit_message>
<xml_diff>
--- a/docs/LCD/customChars.xlsx
+++ b/docs/LCD/customChars.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicot\OneDrive\Documents\MCUXpressoIDE_10.2.0_759\Micros\TPs\tpf-mp3-player\docs\LCD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gonza\Dropbox\My PC (LAPTOP-95UQIM1N)\Desktop\ITBA\LABO_DE_MICROS\tpf-mp3-player\docs\LCD\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D8CC124-7F3E-48DD-852F-A6973492124B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF88CE23-A462-4D3E-81F5-FC856E5F69A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{2621102A-7D8C-481F-A64A-169C19D7CE1B}"/>
+    <workbookView xWindow="-13296" yWindow="888" windowWidth="17280" windowHeight="8964" xr2:uid="{2621102A-7D8C-481F-A64A-169C19D7CE1B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -156,7 +156,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -183,6 +183,14 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -499,13 +507,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{43AA64A4-D781-47F1-9DC0-07FD65ECE894}">
   <dimension ref="A1:AK12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AJ11" sqref="AJ11"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="AM12" sqref="AM12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.9453125" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="3" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:37" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:37" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="3"/>
@@ -524,21 +532,22 @@
       <c r="U1" s="25"/>
       <c r="V1" s="24"/>
       <c r="W1" s="24"/>
-      <c r="X1" s="24"/>
-      <c r="Y1" s="24"/>
-      <c r="Z1" s="24"/>
-      <c r="AA1" s="25"/>
+      <c r="X1" s="26"/>
+      <c r="Y1" s="27"/>
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27"/>
+      <c r="AB1" s="28"/>
       <c r="AC1" s="24"/>
       <c r="AD1" s="24"/>
-      <c r="AE1" s="24"/>
-      <c r="AF1" s="24"/>
-      <c r="AG1" s="24"/>
-      <c r="AH1" s="24"/>
-      <c r="AI1" s="24"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="27"/>
+      <c r="AG1" s="27"/>
+      <c r="AH1" s="27"/>
+      <c r="AI1" s="28"/>
       <c r="AJ1" s="24"/>
       <c r="AK1" s="24"/>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A2" s="5"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -557,21 +566,22 @@
       <c r="U2" s="25"/>
       <c r="V2" s="24"/>
       <c r="W2" s="24"/>
-      <c r="X2" s="24"/>
-      <c r="Y2" s="24"/>
+      <c r="X2" s="29"/>
+      <c r="Y2" s="16"/>
       <c r="Z2" s="24"/>
-      <c r="AA2" s="25"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="30"/>
       <c r="AC2" s="24"/>
       <c r="AD2" s="24"/>
-      <c r="AE2" s="24"/>
-      <c r="AF2" s="24"/>
+      <c r="AE2" s="18"/>
+      <c r="AF2" s="16"/>
       <c r="AG2" s="24"/>
       <c r="AH2" s="24"/>
-      <c r="AI2" s="24"/>
+      <c r="AI2" s="30"/>
       <c r="AJ2" s="24"/>
       <c r="AK2" s="24"/>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A3" s="5"/>
       <c r="B3" s="1"/>
       <c r="C3" s="10"/>
@@ -590,21 +600,22 @@
       <c r="U3" s="25"/>
       <c r="V3" s="24"/>
       <c r="W3" s="24"/>
-      <c r="X3" s="24"/>
-      <c r="Y3" s="24"/>
+      <c r="X3" s="29"/>
+      <c r="Y3" s="16"/>
       <c r="Z3" s="24"/>
-      <c r="AA3" s="25"/>
+      <c r="AA3" s="16"/>
+      <c r="AB3" s="30"/>
       <c r="AC3" s="24"/>
       <c r="AD3" s="24"/>
-      <c r="AE3" s="24"/>
-      <c r="AF3" s="24"/>
-      <c r="AG3" s="24"/>
+      <c r="AE3" s="18"/>
+      <c r="AF3" s="16"/>
+      <c r="AG3" s="16"/>
       <c r="AH3" s="24"/>
-      <c r="AI3" s="24"/>
+      <c r="AI3" s="30"/>
       <c r="AJ3" s="24"/>
       <c r="AK3" s="24"/>
     </row>
-    <row r="4" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A4" s="5"/>
       <c r="B4" s="1"/>
       <c r="C4" s="10"/>
@@ -623,21 +634,22 @@
       <c r="U4" s="25"/>
       <c r="V4" s="24"/>
       <c r="W4" s="24"/>
-      <c r="X4" s="24"/>
-      <c r="Y4" s="24"/>
+      <c r="X4" s="29"/>
+      <c r="Y4" s="16"/>
       <c r="Z4" s="24"/>
-      <c r="AA4" s="25"/>
+      <c r="AA4" s="16"/>
+      <c r="AB4" s="30"/>
       <c r="AC4" s="24"/>
       <c r="AD4" s="24"/>
-      <c r="AE4" s="24"/>
-      <c r="AF4" s="24"/>
-      <c r="AG4" s="24"/>
-      <c r="AH4" s="24"/>
-      <c r="AI4" s="24"/>
+      <c r="AE4" s="18"/>
+      <c r="AF4" s="16"/>
+      <c r="AG4" s="16"/>
+      <c r="AH4" s="16"/>
+      <c r="AI4" s="30"/>
       <c r="AJ4" s="24"/>
       <c r="AK4" s="24"/>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A5" s="8"/>
       <c r="B5" s="1"/>
       <c r="C5" s="10"/>
@@ -656,21 +668,22 @@
       <c r="U5" s="25"/>
       <c r="V5" s="24"/>
       <c r="W5" s="24"/>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="24"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="16"/>
       <c r="Z5" s="24"/>
-      <c r="AA5" s="25"/>
+      <c r="AA5" s="16"/>
+      <c r="AB5" s="30"/>
       <c r="AC5" s="24"/>
       <c r="AD5" s="24"/>
-      <c r="AE5" s="24"/>
-      <c r="AF5" s="24"/>
-      <c r="AG5" s="24"/>
+      <c r="AE5" s="18"/>
+      <c r="AF5" s="16"/>
+      <c r="AG5" s="16"/>
       <c r="AH5" s="24"/>
-      <c r="AI5" s="24"/>
+      <c r="AI5" s="30"/>
       <c r="AJ5" s="24"/>
       <c r="AK5" s="24"/>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A6" s="8"/>
       <c r="B6" s="1"/>
       <c r="C6" s="10"/>
@@ -689,21 +702,22 @@
       <c r="U6" s="25"/>
       <c r="V6" s="24"/>
       <c r="W6" s="24"/>
-      <c r="X6" s="24"/>
-      <c r="Y6" s="24"/>
+      <c r="X6" s="29"/>
+      <c r="Y6" s="16"/>
       <c r="Z6" s="24"/>
-      <c r="AA6" s="25"/>
+      <c r="AA6" s="16"/>
+      <c r="AB6" s="30"/>
       <c r="AC6" s="24"/>
       <c r="AD6" s="24"/>
-      <c r="AE6" s="24"/>
-      <c r="AF6" s="24"/>
+      <c r="AE6" s="18"/>
+      <c r="AF6" s="16"/>
       <c r="AG6" s="24"/>
       <c r="AH6" s="24"/>
-      <c r="AI6" s="24"/>
+      <c r="AI6" s="30"/>
       <c r="AJ6" s="24"/>
       <c r="AK6" s="24"/>
     </row>
-    <row r="7" spans="1:37" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="7" spans="1:37" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="9"/>
       <c r="B7" s="7"/>
       <c r="C7" s="11"/>
@@ -722,21 +736,22 @@
       <c r="U7" s="25"/>
       <c r="V7" s="24"/>
       <c r="W7" s="24"/>
-      <c r="X7" s="24"/>
-      <c r="Y7" s="24"/>
+      <c r="X7" s="29"/>
+      <c r="Y7" s="16"/>
       <c r="Z7" s="24"/>
-      <c r="AA7" s="25"/>
+      <c r="AA7" s="16"/>
+      <c r="AB7" s="30"/>
       <c r="AC7" s="24"/>
       <c r="AD7" s="24"/>
-      <c r="AE7" s="24"/>
+      <c r="AE7" s="18"/>
       <c r="AF7" s="24"/>
       <c r="AG7" s="24"/>
       <c r="AH7" s="24"/>
-      <c r="AI7" s="24"/>
+      <c r="AI7" s="30"/>
       <c r="AJ7" s="24"/>
       <c r="AK7" s="24"/>
     </row>
-    <row r="8" spans="1:37" ht="15" thickTop="1" thickBot="1" x14ac:dyDescent="0.6">
+    <row r="8" spans="1:37" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="I8" s="6"/>
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
@@ -750,21 +765,22 @@
       <c r="U8" s="25"/>
       <c r="V8" s="24"/>
       <c r="W8" s="24"/>
-      <c r="X8" s="24"/>
-      <c r="Y8" s="24"/>
-      <c r="Z8" s="24"/>
-      <c r="AA8" s="25"/>
+      <c r="X8" s="31"/>
+      <c r="Y8" s="32"/>
+      <c r="Z8" s="32"/>
+      <c r="AA8" s="32"/>
+      <c r="AB8" s="33"/>
       <c r="AC8" s="24"/>
       <c r="AD8" s="24"/>
-      <c r="AE8" s="24"/>
-      <c r="AF8" s="24"/>
-      <c r="AG8" s="24"/>
-      <c r="AH8" s="24"/>
-      <c r="AI8" s="24"/>
+      <c r="AE8" s="31"/>
+      <c r="AF8" s="32"/>
+      <c r="AG8" s="32"/>
+      <c r="AH8" s="32"/>
+      <c r="AI8" s="33"/>
       <c r="AJ8" s="24"/>
       <c r="AK8" s="24"/>
     </row>
-    <row r="9" spans="1:37" ht="14.7" thickTop="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:37" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="U9" s="25"/>
       <c r="V9" s="24"/>
       <c r="W9" s="24"/>
@@ -782,7 +798,7 @@
       <c r="AJ9" s="24"/>
       <c r="AK9" s="24"/>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
       <c r="U10" s="25"/>
       <c r="V10" s="24"/>
       <c r="W10" s="24"/>
@@ -800,7 +816,7 @@
       <c r="AJ10" s="24"/>
       <c r="AK10" s="24"/>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
       <c r="AC11" s="24"/>
       <c r="AD11" s="24"/>
       <c r="AE11" s="24"/>
@@ -811,7 +827,7 @@
       <c r="AJ11" s="24"/>
       <c r="AK11" s="24"/>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
       <c r="AC12" s="24"/>
       <c r="AD12" s="24"/>
       <c r="AE12" s="24"/>

</xml_diff>